<commit_message>
ARREGLO HILOS DE LA PROFE
1) Hay un error con las instrucciones, se cambio para arreglarlo (Usa el
R10 en lugar del R4) como se supone en la logica que viene en el excel
</commit_message>
<xml_diff>
--- a/hilos profe/CODIGO HILOS 1ERA PARTE-v2.xlsx
+++ b/hilos profe/CODIGO HILOS 1ERA PARTE-v2.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="217">
   <si>
     <t>Bloque</t>
   </si>
@@ -706,9 +706,6 @@
   </si>
   <si>
     <t>R12= 0+840=840</t>
-  </si>
-  <si>
-    <t>32 12 10 12</t>
   </si>
   <si>
     <t>B21</t>
@@ -1240,7 +1237,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1425,6 +1422,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCC1DA"/>
         <bgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="41"/>
       </patternFill>
     </fill>
   </fills>
@@ -1714,7 +1723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2291,36 +2300,38 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
@@ -2766,8 +2777,8 @@
   </sheetPr>
   <dimension ref="A1:AM86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="C53" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2800,31 +2811,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="230" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="231" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="231"/>
+      <c r="I1" s="231"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="232" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="235" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="235"/>
-      <c r="G1" s="235"/>
-      <c r="H1" s="235"/>
-      <c r="I1" s="235"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="236" t="s">
-        <v>215</v>
-      </c>
-      <c r="L1" s="236"/>
+      <c r="L1" s="232"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -2845,7 +2856,7 @@
       </c>
       <c r="J2" s="157"/>
       <c r="K2" s="226" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L2" s="227"/>
       <c r="O2" s="10"/>
@@ -2863,7 +2874,7 @@
       <c r="AJ2" s="13"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="237" t="s">
+      <c r="A3" s="233" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="14">
@@ -2891,14 +2902,14 @@
       <c r="L3" s="155">
         <v>1</v>
       </c>
-      <c r="O3" s="233"/>
-      <c r="P3" s="233"/>
-      <c r="Q3" s="233"/>
-      <c r="R3" s="233"/>
-      <c r="S3" s="233"/>
-      <c r="T3" s="233"/>
-      <c r="U3" s="233"/>
-      <c r="V3" s="233"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="228"/>
+      <c r="Q3" s="228"/>
+      <c r="R3" s="228"/>
+      <c r="S3" s="228"/>
+      <c r="T3" s="228"/>
+      <c r="U3" s="228"/>
+      <c r="V3" s="228"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="13"/>
       <c r="AD3" s="13"/>
@@ -2906,7 +2917,7 @@
       <c r="AK3" s="13"/>
     </row>
     <row r="4" spans="1:39" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
+      <c r="A4" s="233"/>
       <c r="B4" s="22">
         <f t="shared" ref="B4:B35" si="0">B3+4</f>
         <v>4</v>
@@ -2934,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
@@ -2951,7 +2962,7 @@
       <c r="AK4" s="13"/>
     </row>
     <row r="5" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
+      <c r="A5" s="233"/>
       <c r="B5" s="22">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3009,7 +3020,7 @@
       <c r="AM5" s="36"/>
     </row>
     <row r="6" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
+      <c r="A6" s="233"/>
       <c r="B6" s="22">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3067,7 +3078,7 @@
       <c r="AM6" s="36"/>
     </row>
     <row r="7" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="237" t="s">
+      <c r="A7" s="233" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="22">
@@ -3127,7 +3138,7 @@
       <c r="AM7" s="36"/>
     </row>
     <row r="8" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="237" t="s">
+      <c r="A8" s="233" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="22">
@@ -3189,7 +3200,7 @@
       <c r="AM8" s="36"/>
     </row>
     <row r="9" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="237"/>
+      <c r="A9" s="233"/>
       <c r="B9" s="22">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3245,7 +3256,7 @@
       <c r="AM9" s="36"/>
     </row>
     <row r="10" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="237" t="s">
+      <c r="A10" s="233" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="22">
@@ -3303,7 +3314,7 @@
       <c r="AM10" s="36"/>
     </row>
     <row r="11" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="237" t="s">
+      <c r="A11" s="233" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22">
@@ -3363,7 +3374,7 @@
       <c r="AM11" s="36"/>
     </row>
     <row r="12" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="237" t="s">
+      <c r="A12" s="233" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="22">
@@ -3417,7 +3428,7 @@
       <c r="AM12" s="36"/>
     </row>
     <row r="13" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="237"/>
+      <c r="A13" s="233"/>
       <c r="B13" s="22">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3469,7 +3480,7 @@
       <c r="AM13" s="36"/>
     </row>
     <row r="14" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="237" t="s">
+      <c r="A14" s="233" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="22">
@@ -3523,7 +3534,7 @@
       <c r="AM14" s="36"/>
     </row>
     <row r="15" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="233" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="22">
@@ -3575,7 +3586,7 @@
       <c r="AM15" s="36"/>
     </row>
     <row r="16" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="237" t="s">
+      <c r="A16" s="233" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="22">
@@ -3631,7 +3642,7 @@
       <c r="AM16" s="36"/>
     </row>
     <row r="17" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="237"/>
+      <c r="A17" s="233"/>
       <c r="B17" s="22">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3647,7 +3658,7 @@
         <v>76</v>
       </c>
       <c r="G17" s="154" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="39"/>
@@ -3683,7 +3694,7 @@
       <c r="AM17" s="36"/>
     </row>
     <row r="18" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="237" t="s">
+      <c r="A18" s="233" t="s">
         <v>77</v>
       </c>
       <c r="B18" s="22">
@@ -3737,7 +3748,7 @@
       <c r="AM18" s="36"/>
     </row>
     <row r="19" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="230" t="s">
+      <c r="A19" s="229" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="43">
@@ -3795,7 +3806,7 @@
       <c r="AM19" s="36"/>
     </row>
     <row r="20" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="230"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="49">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3808,7 +3819,7 @@
         <v>84</v>
       </c>
       <c r="F20" s="224" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G20" s="53" t="s">
         <v>85</v>
@@ -3817,7 +3828,7 @@
       <c r="I20" s="54"/>
       <c r="J20" s="162"/>
       <c r="K20" s="172" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L20" s="173">
         <v>2</v>
@@ -3851,7 +3862,7 @@
       <c r="AM20" s="36"/>
     </row>
     <row r="21" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="230"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="49">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -3907,7 +3918,7 @@
       <c r="AM21" s="36"/>
     </row>
     <row r="22" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="230"/>
+      <c r="A22" s="229"/>
       <c r="B22" s="49">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -3922,7 +3933,7 @@
         <v>91</v>
       </c>
       <c r="F22" s="224" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G22" s="53" t="s">
         <v>92</v>
@@ -3965,7 +3976,7 @@
       <c r="AM22" s="36"/>
     </row>
     <row r="23" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="230" t="s">
+      <c r="A23" s="229" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="49">
@@ -4025,7 +4036,7 @@
       <c r="AM23" s="36"/>
     </row>
     <row r="24" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="230" t="s">
+      <c r="A24" s="229" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="49">
@@ -4085,7 +4096,7 @@
       <c r="AM24" s="36"/>
     </row>
     <row r="25" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="230"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="49">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -4109,7 +4120,7 @@
       </c>
       <c r="J25" s="163"/>
       <c r="K25" s="172" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L25" s="173">
         <v>0</v>
@@ -4143,7 +4154,7 @@
       <c r="AM25" s="36"/>
     </row>
     <row r="26" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="230" t="s">
+      <c r="A26" s="229" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="49">
@@ -4158,7 +4169,7 @@
         <v>104</v>
       </c>
       <c r="F26" s="224" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G26" s="53" t="s">
         <v>105</v>
@@ -4203,7 +4214,7 @@
       <c r="AM26" s="36"/>
     </row>
     <row r="27" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="230" t="s">
+      <c r="A27" s="229" t="s">
         <v>70</v>
       </c>
       <c r="B27" s="49">
@@ -4255,7 +4266,7 @@
       <c r="AM27" s="36"/>
     </row>
     <row r="28" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="230" t="s">
+      <c r="A28" s="229" t="s">
         <v>107</v>
       </c>
       <c r="B28" s="49">
@@ -4311,7 +4322,7 @@
       <c r="AM28" s="36"/>
     </row>
     <row r="29" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="230"/>
+      <c r="A29" s="229"/>
       <c r="B29" s="49">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -4363,7 +4374,7 @@
       <c r="AM29" s="36"/>
     </row>
     <row r="30" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="230" t="s">
+      <c r="A30" s="229" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="49">
@@ -4417,7 +4428,7 @@
       <c r="AM30" s="36"/>
     </row>
     <row r="31" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="230" t="s">
+      <c r="A31" s="229" t="s">
         <v>77</v>
       </c>
       <c r="B31" s="49">
@@ -4473,7 +4484,7 @@
       <c r="AM31" s="36"/>
     </row>
     <row r="32" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="230" t="s">
+      <c r="A32" s="229" t="s">
         <v>122</v>
       </c>
       <c r="B32" s="49">
@@ -4527,7 +4538,7 @@
       <c r="AM32" s="36"/>
     </row>
     <row r="33" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="230"/>
+      <c r="A33" s="229"/>
       <c r="B33" s="49">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -4579,7 +4590,7 @@
       <c r="AM33" s="36"/>
     </row>
     <row r="34" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="230" t="s">
+      <c r="A34" s="229" t="s">
         <v>129</v>
       </c>
       <c r="B34" s="49">
@@ -4941,14 +4952,14 @@
       </c>
       <c r="J42" s="166"/>
       <c r="K42" s="187" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L42" s="188">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="231" t="s">
+      <c r="A43" s="236" t="s">
         <v>98</v>
       </c>
       <c r="B43" s="88">
@@ -4972,14 +4983,14 @@
       <c r="I43" s="85"/>
       <c r="J43" s="166"/>
       <c r="K43" s="187" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L43" s="188">
         <v>1688</v>
       </c>
     </row>
     <row r="44" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="231" t="s">
+      <c r="A44" s="236" t="s">
         <v>159</v>
       </c>
       <c r="B44" s="88">
@@ -5005,14 +5016,14 @@
       </c>
       <c r="J44" s="166"/>
       <c r="K44" s="189" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L44" s="190">
         <v>5064</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A45" s="231"/>
+      <c r="A45" s="236"/>
       <c r="B45" s="88">
         <f t="shared" si="1"/>
         <v>168</v>
@@ -5027,8 +5038,8 @@
       <c r="F45" s="91" t="s">
         <v>162</v>
       </c>
-      <c r="G45" s="96" t="s">
-        <v>163</v>
+      <c r="G45" s="238" t="s">
+        <v>166</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="98"/>
@@ -5037,8 +5048,8 @@
       <c r="L45" s="183"/>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A46" s="231" t="s">
-        <v>164</v>
+      <c r="A46" s="236" t="s">
+        <v>163</v>
       </c>
       <c r="B46" s="88">
         <f t="shared" si="1"/>
@@ -5052,7 +5063,7 @@
         <v>40</v>
       </c>
       <c r="F46" s="91" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G46" s="96" t="s">
         <v>42</v>
@@ -5077,10 +5088,10 @@
         <v>161</v>
       </c>
       <c r="F47" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" s="96" t="s">
         <v>166</v>
-      </c>
-      <c r="G47" s="96" t="s">
-        <v>167</v>
       </c>
       <c r="H47" s="27"/>
       <c r="I47" s="100"/>
@@ -5101,13 +5112,13 @@
         <v>50</v>
       </c>
       <c r="E48" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="F48" s="91" t="s">
+      <c r="G48" s="96" t="s">
         <v>169</v>
-      </c>
-      <c r="G48" s="96" t="s">
-        <v>170</v>
       </c>
       <c r="H48" s="27"/>
       <c r="I48" s="100"/>
@@ -5127,7 +5138,7 @@
       </c>
       <c r="E49" s="103"/>
       <c r="F49" s="91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G49" s="96" t="s">
         <v>69</v>
@@ -5168,7 +5179,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="232" t="s">
+      <c r="A51" s="237" t="s">
         <v>107</v>
       </c>
       <c r="B51" s="112">
@@ -5199,7 +5210,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="232"/>
+      <c r="A52" s="237"/>
       <c r="B52" s="113">
         <f t="shared" si="1"/>
         <v>196</v>
@@ -5228,7 +5239,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="232"/>
+      <c r="A53" s="237"/>
       <c r="B53" s="112">
         <f t="shared" si="1"/>
         <v>200</v>
@@ -5259,7 +5270,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="232"/>
+      <c r="A54" s="237"/>
       <c r="B54" s="112">
         <f t="shared" si="1"/>
         <v>204</v>
@@ -5290,7 +5301,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="232" t="s">
+      <c r="A55" s="237" t="s">
         <v>114</v>
       </c>
       <c r="B55" s="112">
@@ -5325,8 +5336,8 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="232" t="s">
-        <v>172</v>
+      <c r="A56" s="237" t="s">
+        <v>171</v>
       </c>
       <c r="B56" s="112">
         <f t="shared" si="1"/>
@@ -5358,7 +5369,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="232"/>
+      <c r="A57" s="237"/>
       <c r="B57" s="112">
         <f t="shared" si="1"/>
         <v>216</v>
@@ -5368,7 +5379,7 @@
         <v>45</v>
       </c>
       <c r="E57" s="119" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F57" s="120" t="s">
         <v>47</v>
@@ -5387,8 +5398,8 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="232" t="s">
-        <v>174</v>
+      <c r="A58" s="237" t="s">
+        <v>173</v>
       </c>
       <c r="B58" s="112">
         <f t="shared" si="1"/>
@@ -5420,7 +5431,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="232" t="s">
+      <c r="A59" s="237" t="s">
         <v>122</v>
       </c>
       <c r="B59" s="112">
@@ -5447,8 +5458,8 @@
       <c r="L59" s="193"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="232" t="s">
-        <v>175</v>
+      <c r="A60" s="237" t="s">
+        <v>174</v>
       </c>
       <c r="B60" s="112">
         <f t="shared" si="1"/>
@@ -5462,7 +5473,7 @@
         <v>8</v>
       </c>
       <c r="F60" s="109" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G60" s="121" t="s">
         <v>61</v>
@@ -5474,7 +5485,7 @@
       <c r="L60" s="195"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="232"/>
+      <c r="A61" s="237"/>
       <c r="B61" s="112">
         <f t="shared" si="1"/>
         <v>232</v>
@@ -5487,7 +5498,7 @@
         <v>64</v>
       </c>
       <c r="F61" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G61" s="121" t="s">
         <v>66</v>
@@ -5499,8 +5510,8 @@
       <c r="L61" s="195"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="232" t="s">
-        <v>177</v>
+      <c r="A62" s="237" t="s">
+        <v>176</v>
       </c>
       <c r="B62" s="112">
         <f t="shared" si="1"/>
@@ -5512,7 +5523,7 @@
       </c>
       <c r="E62" s="119"/>
       <c r="F62" s="120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G62" s="121" t="s">
         <v>69</v>
@@ -5563,13 +5574,13 @@
         <v>45</v>
       </c>
       <c r="E64" s="119" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F64" s="120" t="s">
         <v>76</v>
       </c>
       <c r="G64" s="154" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H64" s="27"/>
       <c r="I64" s="111"/>
@@ -5632,8 +5643,8 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="228" t="s">
-        <v>179</v>
+      <c r="A67" s="234" t="s">
+        <v>178</v>
       </c>
       <c r="B67" s="134">
         <f t="shared" si="1"/>
@@ -5663,8 +5674,8 @@
       </c>
     </row>
     <row r="68" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="228" t="s">
-        <v>180</v>
+      <c r="A68" s="234" t="s">
+        <v>179</v>
       </c>
       <c r="B68" s="136">
         <f t="shared" ref="B68:B86" si="2">B67+4</f>
@@ -5696,7 +5707,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="228"/>
+      <c r="A69" s="234"/>
       <c r="B69" s="136">
         <f t="shared" si="2"/>
         <v>264</v>
@@ -5727,8 +5738,8 @@
       </c>
     </row>
     <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="228" t="s">
-        <v>181</v>
+      <c r="A70" s="234" t="s">
+        <v>180</v>
       </c>
       <c r="B70" s="136">
         <f t="shared" si="2"/>
@@ -5753,15 +5764,15 @@
       </c>
       <c r="J70" s="207"/>
       <c r="K70" s="203" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L70" s="204">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="228" t="s">
-        <v>182</v>
+      <c r="A71" s="234" t="s">
+        <v>181</v>
       </c>
       <c r="B71" s="136">
         <f t="shared" si="2"/>
@@ -5786,15 +5797,15 @@
       </c>
       <c r="J71" s="207"/>
       <c r="K71" s="203" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L71" s="204">
         <v>1688</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="228" t="s">
-        <v>183</v>
+      <c r="A72" s="234" t="s">
+        <v>182</v>
       </c>
       <c r="B72" s="136">
         <f t="shared" si="2"/>
@@ -5817,14 +5828,14 @@
       <c r="I72" s="137"/>
       <c r="J72" s="207"/>
       <c r="K72" s="203" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L72" s="204">
         <v>5064</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="228"/>
+      <c r="A73" s="234"/>
       <c r="B73" s="136">
         <f t="shared" si="2"/>
         <v>280</v>
@@ -5839,8 +5850,8 @@
       <c r="F73" s="130" t="s">
         <v>162</v>
       </c>
-      <c r="G73" s="131" t="s">
-        <v>163</v>
+      <c r="G73" s="239" t="s">
+        <v>166</v>
       </c>
       <c r="H73" s="27"/>
       <c r="I73" s="137">
@@ -5851,8 +5862,8 @@
       <c r="L73" s="212"/>
     </row>
     <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="228" t="s">
-        <v>184</v>
+      <c r="A74" s="234" t="s">
+        <v>183</v>
       </c>
       <c r="B74" s="136">
         <f t="shared" si="2"/>
@@ -5866,7 +5877,7 @@
         <v>40</v>
       </c>
       <c r="F74" s="130" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G74" s="131" t="s">
         <v>42</v>
@@ -5891,10 +5902,10 @@
         <v>161</v>
       </c>
       <c r="F75" s="130" t="s">
+        <v>165</v>
+      </c>
+      <c r="G75" s="131" t="s">
         <v>166</v>
-      </c>
-      <c r="G75" s="131" t="s">
-        <v>167</v>
       </c>
       <c r="H75" s="27"/>
       <c r="I75" s="137"/>
@@ -5904,7 +5915,7 @@
     </row>
     <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="139" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B76" s="136">
         <f t="shared" si="2"/>
@@ -5915,13 +5926,13 @@
         <v>50</v>
       </c>
       <c r="E76" s="129" t="s">
+        <v>167</v>
+      </c>
+      <c r="F76" s="130" t="s">
         <v>168</v>
       </c>
-      <c r="F76" s="130" t="s">
+      <c r="G76" s="131" t="s">
         <v>169</v>
-      </c>
-      <c r="G76" s="131" t="s">
-        <v>170</v>
       </c>
       <c r="H76" s="27"/>
       <c r="I76" s="137"/>
@@ -5941,7 +5952,7 @@
       </c>
       <c r="E77" s="129"/>
       <c r="F77" s="130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G77" s="131" t="s">
         <v>69</v>
@@ -5963,7 +5974,7 @@
         <v>7</v>
       </c>
       <c r="E78" s="144" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F78" s="145" t="s">
         <v>9</v>
@@ -5982,8 +5993,8 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="229" t="s">
-        <v>188</v>
+      <c r="A79" s="235" t="s">
+        <v>187</v>
       </c>
       <c r="B79" s="149">
         <f t="shared" si="2"/>
@@ -5994,13 +6005,13 @@
         <v>7</v>
       </c>
       <c r="E79" s="144" t="s">
+        <v>188</v>
+      </c>
+      <c r="F79" s="145" t="s">
         <v>189</v>
       </c>
-      <c r="F79" s="145" t="s">
+      <c r="G79" s="146" t="s">
         <v>190</v>
-      </c>
-      <c r="G79" s="146" t="s">
-        <v>191</v>
       </c>
       <c r="H79" s="27"/>
       <c r="I79" s="148"/>
@@ -6013,7 +6024,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="229"/>
+      <c r="A80" s="235"/>
       <c r="B80" s="149">
         <f t="shared" si="2"/>
         <v>308</v>
@@ -6044,8 +6055,8 @@
       </c>
     </row>
     <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="229" t="s">
-        <v>192</v>
+      <c r="A81" s="235" t="s">
+        <v>191</v>
       </c>
       <c r="B81" s="149">
         <f t="shared" si="2"/>
@@ -6077,7 +6088,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="229"/>
+      <c r="A82" s="235"/>
       <c r="B82" s="149">
         <f t="shared" si="2"/>
         <v>316</v>
@@ -6087,13 +6098,13 @@
         <v>7</v>
       </c>
       <c r="E82" s="144" t="s">
+        <v>192</v>
+      </c>
+      <c r="F82" s="145" t="s">
         <v>193</v>
       </c>
-      <c r="F82" s="145" t="s">
+      <c r="G82" s="146" t="s">
         <v>194</v>
-      </c>
-      <c r="G82" s="146" t="s">
-        <v>195</v>
       </c>
       <c r="H82" s="27"/>
       <c r="I82" s="148" t="s">
@@ -6101,14 +6112,14 @@
       </c>
       <c r="J82" s="214"/>
       <c r="K82" s="222" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L82" s="223">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="229" t="s">
+      <c r="A83" s="235" t="s">
         <v>159</v>
       </c>
       <c r="B83" s="149">
@@ -6125,7 +6136,7 @@
         <v>34</v>
       </c>
       <c r="F83" s="145" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G83" s="146" t="s">
         <v>36</v>
@@ -6139,7 +6150,7 @@
       <c r="L83" s="216"/>
     </row>
     <row r="84" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="229"/>
+      <c r="A84" s="235"/>
       <c r="B84" s="149">
         <f t="shared" si="2"/>
         <v>324</v>
@@ -6152,7 +6163,7 @@
         <v>40</v>
       </c>
       <c r="F84" s="145" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G84" s="146" t="s">
         <v>42</v>
@@ -6164,8 +6175,8 @@
       <c r="L84" s="216"/>
     </row>
     <row r="85" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="229" t="s">
-        <v>198</v>
+      <c r="A85" s="235" t="s">
+        <v>197</v>
       </c>
       <c r="B85" s="149">
         <f t="shared" si="2"/>
@@ -6176,10 +6187,10 @@
         <v>45</v>
       </c>
       <c r="E85" s="144" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F85" s="145" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G85" s="146" t="s">
         <v>48</v>
@@ -6193,7 +6204,7 @@
       <c r="L85" s="216"/>
     </row>
     <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="229"/>
+      <c r="A86" s="235"/>
       <c r="B86" s="149">
         <f t="shared" si="2"/>
         <v>332</v>
@@ -6204,7 +6215,7 @@
       </c>
       <c r="E86" s="144"/>
       <c r="F86" s="145" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G86" s="146" t="s">
         <v>69</v>
@@ -6218,6 +6229,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="21">
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A67:A70"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="R3:V3"/>
     <mergeCell ref="A27:A30"/>
@@ -6230,15 +6250,6 @@
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A67:A70"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
   <pageMargins left="0.23" right="0.14000000000000001" top="0.24027777777777778" bottom="0.16" header="0.27" footer="0.51180555555555551"/>

</xml_diff>